<commit_message>
adjusted team names in the ranking df
</commit_message>
<xml_diff>
--- a/unified_ranking_data.xlsx
+++ b/unified_ranking_data.xlsx
@@ -622,7 +622,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>aa gent</t>
+          <t>kaa gent</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -667,7 +667,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>aab aalborg</t>
+          <t>aalborg bk</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1419,7 +1419,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ajax</t>
+          <t>afc ajax</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1684,7 +1684,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>anderlecht</t>
+          <t>rsc anderlecht</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1895,7 +1895,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>apoel nicosia</t>
+          <t>apoel nikosia</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2122,7 +2122,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>arsenal</t>
+          <t>arsenal fc</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2683,7 +2683,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>atlético madrid</t>
+          <t>atletico madrid</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -3305,7 +3305,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>bayer leverkusen</t>
+          <t>bayer 04 leverkusen</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3560,7 +3560,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>benfica</t>
+          <t>sl benfica</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3648,7 +3648,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>besiktas</t>
+          <t>beşiktaş i̇stanbul jk</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3908,7 +3908,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>boavista</t>
+          <t>boavista fc</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -4142,7 +4142,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>borussia mönchengladbach</t>
+          <t>borussia monchengladbach</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -4591,7 +4591,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>celta de vigo</t>
+          <t>celta vigo</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -4636,7 +4636,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>celtic</t>
+          <t>celtic fc</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -4819,7 +4819,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>chelsea</t>
+          <t>chelsea fc</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -5431,7 +5431,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>cska moscow</t>
+          <t>cska moskva</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -5914,7 +5914,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>deportivo la coruña</t>
+          <t>deportivo la coruna</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -6795,7 +6795,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>dvsc debrecen</t>
+          <t>debreceni vsc</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -7862,7 +7862,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>fc basel</t>
+          <t>basel</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -8123,7 +8123,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>fc københavn</t>
+          <t>kobenhavn</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -8427,7 +8427,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>fc nordsjælland</t>
+          <t>nordsjaelland</t>
         </is>
       </c>
       <c r="B194" t="inlineStr"/>
@@ -8814,7 +8814,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>fc thun</t>
+          <t>thun</t>
         </is>
       </c>
       <c r="B203" t="inlineStr"/>
@@ -8970,7 +8970,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>fc twente enschede</t>
+          <t>fc twente</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -9201,7 +9201,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>fc zürich</t>
+          <t>fc zurich</t>
         </is>
       </c>
       <c r="B212" t="inlineStr"/>
@@ -9271,7 +9271,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>fenerbahçe</t>
+          <t>fenerbahçe i̇stanbul sk</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -9371,7 +9371,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>feyenoord</t>
+          <t>feyenoord rotterdam</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -9536,7 +9536,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>fiorentina</t>
+          <t>acf fiorentina</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -9636,7 +9636,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>fk astana</t>
+          <t>astana</t>
         </is>
       </c>
       <c r="B221" t="inlineStr"/>
@@ -11013,7 +11013,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>galatasaray</t>
+          <t>galatasaray i̇stanbul aş</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -11599,7 +11599,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>glasgow rangers</t>
+          <t>rangers fc</t>
         </is>
       </c>
       <c r="B272" t="n">
@@ -12323,7 +12323,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>hapoel tel-aviv</t>
+          <t>hapoel tel aviv</t>
         </is>
       </c>
       <c r="B290" t="n">
@@ -12478,7 +12478,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>heerenveen</t>
+          <t>sc heerenveen</t>
         </is>
       </c>
       <c r="B293" t="n">
@@ -12533,7 +12533,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>helsingborg if</t>
+          <t>helsingborgs if</t>
         </is>
       </c>
       <c r="B294" t="n">
@@ -15237,7 +15237,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>lazio</t>
+          <t>ss lazio</t>
         </is>
       </c>
       <c r="B362" t="n">
@@ -15337,7 +15337,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>leeds united</t>
+          <t>leeds united fc</t>
         </is>
       </c>
       <c r="B364" t="n">
@@ -16044,7 +16044,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>liverpool</t>
+          <t>liverpool fc</t>
         </is>
       </c>
       <c r="B381" t="n">
@@ -16235,7 +16235,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>lokomotiv moscow</t>
+          <t>lokomotiv moskva</t>
         </is>
       </c>
       <c r="B386" t="n">
@@ -16438,7 +16438,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>ludogorets razgrad</t>
+          <t>pfc ludogorets razgrad</t>
         </is>
       </c>
       <c r="B391" t="inlineStr"/>
@@ -16692,7 +16692,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>maccabi tel-aviv</t>
+          <t>maccabi tel aviv</t>
         </is>
       </c>
       <c r="B397" t="n">
@@ -16803,7 +16803,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>malmö ff</t>
+          <t>malmo ff</t>
         </is>
       </c>
       <c r="B400" t="inlineStr"/>
@@ -16897,7 +16897,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>manchester city</t>
+          <t>manchester city fc</t>
         </is>
       </c>
       <c r="B402" t="n">
@@ -16952,7 +16952,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>manchester united</t>
+          <t>manchester united fc</t>
         </is>
       </c>
       <c r="B403" t="n">
@@ -17853,7 +17853,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>montpellier</t>
+          <t>montpellier hsc</t>
         </is>
       </c>
       <c r="B424" t="inlineStr"/>
@@ -18136,7 +18136,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>málaga cf</t>
+          <t>malaga cf</t>
         </is>
       </c>
       <c r="B431" t="n">
@@ -18304,7 +18304,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>napoli</t>
+          <t>ssc napoli</t>
         </is>
       </c>
       <c r="B435" t="inlineStr"/>
@@ -18639,7 +18639,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>newcastle united</t>
+          <t>newcastle united fc</t>
         </is>
       </c>
       <c r="B444" t="n">
@@ -19785,7 +19785,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>olympiakos piraeus</t>
+          <t>olympiacos</t>
         </is>
       </c>
       <c r="B472" t="n">
@@ -20230,7 +20230,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>panathinaikos</t>
+          <t>panathinaikos fc</t>
         </is>
       </c>
       <c r="B483" t="n">
@@ -20759,7 +20759,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>petrzalka bratislava</t>
+          <t>petrzalka akademia</t>
         </is>
       </c>
       <c r="B496" t="n">
@@ -21372,7 +21372,7 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>racing genk</t>
+          <t>krc genk</t>
         </is>
       </c>
       <c r="B511" t="n">
@@ -21814,7 +21814,7 @@
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>real madrid</t>
+          <t>real madrid cf</t>
         </is>
       </c>
       <c r="B521" t="n">
@@ -21869,7 +21869,7 @@
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>real mallorca</t>
+          <t>rcd mallorca</t>
         </is>
       </c>
       <c r="B522" t="n">
@@ -22887,7 +22887,7 @@
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>schalke 04</t>
+          <t>fc schalke 04</t>
         </is>
       </c>
       <c r="B548" t="n">
@@ -23122,7 +23122,7 @@
     <row r="553">
       <c r="A553" t="inlineStr">
         <is>
-          <t>sevilla</t>
+          <t>sevilla fc</t>
         </is>
       </c>
       <c r="B553" t="n">
@@ -24570,7 +24570,7 @@
     <row r="589">
       <c r="A589" t="inlineStr">
         <is>
-          <t>spartak moscow</t>
+          <t>spartak moskva</t>
         </is>
       </c>
       <c r="B589" t="n">
@@ -24833,7 +24833,7 @@
     <row r="596">
       <c r="A596" t="inlineStr">
         <is>
-          <t>sporting cp lisbon</t>
+          <t>sporting cp</t>
         </is>
       </c>
       <c r="B596" t="n">
@@ -25134,7 +25134,7 @@
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>standard liège</t>
+          <t>standard liege</t>
         </is>
       </c>
       <c r="B603" t="n">
@@ -25347,7 +25347,7 @@
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>sturm graz</t>
+          <t>sk sturm graz</t>
         </is>
       </c>
       <c r="B608" t="n">
@@ -26158,7 +26158,7 @@
     <row r="629">
       <c r="A629" t="inlineStr">
         <is>
-          <t>tottenham hotspur</t>
+          <t>tottenham hotspur fc</t>
         </is>
       </c>
       <c r="B629" t="inlineStr"/>
@@ -26271,7 +26271,7 @@
     <row r="632">
       <c r="A632" t="inlineStr">
         <is>
-          <t>trabzonspor</t>
+          <t>trabzonspor aş</t>
         </is>
       </c>
       <c r="B632" t="n">
@@ -26601,7 +26601,7 @@
     <row r="640">
       <c r="A640" t="inlineStr">
         <is>
-          <t>udinese</t>
+          <t>udinese calcio</t>
         </is>
       </c>
       <c r="B640" t="n">
@@ -27001,7 +27001,7 @@
     <row r="650">
       <c r="A650" t="inlineStr">
         <is>
-          <t>valencia</t>
+          <t>valencia cf</t>
         </is>
       </c>
       <c r="B650" t="n">
@@ -27661,7 +27661,7 @@
     <row r="668">
       <c r="A668" t="inlineStr">
         <is>
-          <t>villarreal</t>
+          <t>villarreal cf</t>
         </is>
       </c>
       <c r="B668" t="n">

</xml_diff>